<commit_message>
Test cases and some automation tests added
</commit_message>
<xml_diff>
--- a/Tasks A and B.xlsx
+++ b/Tasks A and B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\Posao\TraceLabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CD5FE0-8B44-4776-840F-E4093A90ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D196202-9DA2-4D0E-8CCE-3E2F25F1F1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C726E65B-F139-476B-A723-A8B2646C1BBD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Test Scenario Template</t>
   </si>
@@ -46,40 +46,28 @@
     <t>Test Scenario Description</t>
   </si>
   <si>
-    <t>Verify that you can not register with all blank fields</t>
-  </si>
-  <si>
-    <t>Verify that you can not register with any blank field</t>
-  </si>
-  <si>
-    <t>Verify that all fields have placeholder as per requirements</t>
-  </si>
-  <si>
-    <t>Verify that you can not use symbols in username field</t>
-  </si>
-  <si>
-    <t>Verify that you can not register without checking Terms and Conditions checkbox</t>
-  </si>
-  <si>
-    <t>Verify that you can not register with different conformation fields (email address and/or password)</t>
-  </si>
-  <si>
-    <t>Verify that you can not register without checking reCAPTCHA iframe</t>
-  </si>
-  <si>
-    <t>Verify that you can successfully register with all fields fulfilled with data as per requirements</t>
-  </si>
-  <si>
-    <t>Check edge cases (username with 4,5,30 and 31 length)</t>
-  </si>
-  <si>
-    <t>Verify that you can (not) register without checking subscription checkbox</t>
-  </si>
-  <si>
     <t>I can put thread.sleep and solve captcha by myself to successfully register, but it is not 100% automated.</t>
   </si>
   <si>
     <t>For these scenarios I would use Selenium because of the huge number of libraries that can help us automate tests. I prefer writing codes in Java language, in IntelliJ Idea. The only problem for automation of this registration form is reCAPTCHA. I can catch iframe, and check it, but most of the time after that, pictures appear and I solving that captcha problem is out of my knowledge right now.</t>
+  </si>
+  <si>
+    <t>Verify that you can successfully register with only mandatory fields filed in correctly</t>
+  </si>
+  <si>
+    <t>Verify that you can successfully register with all fields filled in correctly</t>
+  </si>
+  <si>
+    <t>Verify that you can not register with all mandatory fields filled in incorrectly (or blank)</t>
+  </si>
+  <si>
+    <t>Verify that you can not register with all fields filled in incorrectly (or blank)</t>
+  </si>
+  <si>
+    <t>Verify that all the fields have placeholders as per documentation</t>
+  </si>
+  <si>
+    <t>Verify that Terms and Conditions and Unsubscribe hyperlinks are working correctly</t>
   </si>
 </sst>
 </file>
@@ -474,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0F7172-8787-4787-B2E1-628C3FC8FCC2}">
-  <dimension ref="A2:B17"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,89 +492,57 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>13</v>
+      <c r="B13" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit about tools i'd use
</commit_message>
<xml_diff>
--- a/Tasks A and B.xlsx
+++ b/Tasks A and B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\Posao\TraceLabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D196202-9DA2-4D0E-8CCE-3E2F25F1F1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B778FEF5-E907-4A3C-AD60-7818B95B9F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C726E65B-F139-476B-A723-A8B2646C1BBD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Test Scenario Template</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Verify that Terms and Conditions and Unsubscribe hyperlinks are working correctly</t>
+  </si>
+  <si>
+    <t>For test scenarios and test cases I would rather use Jira, TestRail or some other testing management tool.</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0F7172-8787-4787-B2E1-628C3FC8FCC2}">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,13 +538,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>